<commit_message>
update CV.pdf & Excel
</commit_message>
<xml_diff>
--- a/download/CV_PedroRios_2020_bis.xlsx
+++ b/download/CV_PedroRios_2020_bis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\CV2022\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D4DE0CD-FB31-4AC8-A66B-2CD742EF7EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0F60FD-2B62-415A-880E-5B6CAB3246C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>Pedro RIOS MACIAS</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>https://cvpedrorios.netlify.app</t>
+  </si>
+  <si>
+    <t>Actualidad</t>
   </si>
 </sst>
 </file>
@@ -460,14 +463,14 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -889,7 +892,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6783915" y="9203091"/>
-          <a:ext cx="1291167" cy="353659"/>
+          <a:ext cx="1291167" cy="385409"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1166,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1370,17 +1373,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="5">
+    <row r="52" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="5">
         <v>2022</v>
       </c>
-      <c r="D52" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="5"/>
-      <c r="D53" s="16"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
@@ -1622,14 +1627,14 @@
       <c r="B106" s="10"/>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D129" s="14" t="s">
+      <c r="D129" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E129" s="15"/>
+      <c r="E129" s="17"/>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D130" s="15"/>
-      <c r="E130" s="15"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C132" s="8"/>

</xml_diff>